<commit_message>
RDCC-2470 handle trimming in role mapping file
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/ServiceRoleMapping_BBA9_extra_spaces.xlsx
+++ b/src/integrationTest/resources/ServiceRoleMapping_BBA9_extra_spaces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/429962/hmcts/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CF054-F0F1-4546-8943-7AAF84130CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA57944-201D-5E4F-8542-5B558EC4FE5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Service ID</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve"> caseworker-iac-bulkscan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBA9 </t>
   </si>
 </sst>
 </file>
@@ -415,16 +418,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EC9574-42D9-2D49-9FE6-FC22AA6AFF8E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -473,12 +476,23 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>